<commit_message>
Enable masive invoice load
</commit_message>
<xml_diff>
--- a/invoice-manager-services/src/main/resources/samples/FormatoMuestra.xlsx
+++ b/invoice-manager-services/src/main/resources/samples/FormatoMuestra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hha0009/development/java/ppt-platform/invoice-manager-services/src/main/resources/samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\ppt-platform\invoice-manager-services\src\main\resources\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31449425-F30E-F643-B163-7467E200BA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CD499B-5EED-4F65-9F36-8833B87926A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="1600" windowWidth="28620" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="-15075" windowWidth="26220" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CARGA_MASIVA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -63,9 +63,6 @@
     <t>476</t>
   </si>
   <si>
-    <t>AXKAN PUBLICIDAD SA DE CV</t>
-  </si>
-  <si>
     <t>SERVICIO</t>
   </si>
   <si>
@@ -75,48 +72,27 @@
     <t xml:space="preserve">COMISIÓN POR INTERMEDIACIÓN Y COLOCACIÓN DE LA OPERACIÓN </t>
   </si>
   <si>
-    <t>NOPRAVO MEXICO SA DE CV</t>
-  </si>
-  <si>
     <t>477</t>
   </si>
   <si>
-    <t xml:space="preserve">CORPORACION MEXICANA DE ESTRATEGIAS COMERCIALES NUVARA SA DE CV </t>
-  </si>
-  <si>
     <t>TAPIZ PENELOPE.</t>
   </si>
   <si>
-    <t xml:space="preserve">DOTACIONES Y SUMINISTROS XALOM SA DE CV </t>
-  </si>
-  <si>
     <t>478</t>
   </si>
   <si>
-    <t>GREBA MARKETING SA DE CV</t>
-  </si>
-  <si>
     <t>Servicios de Publicidad enfocados en realizar estudios de mercado, estrategias comerciales y difusión en medios de servicios comerciales.</t>
   </si>
   <si>
     <t>PPD</t>
   </si>
   <si>
-    <t xml:space="preserve">ASESORES EN PUBLICIDAD VICEY SA DE CV   </t>
-  </si>
-  <si>
     <t>479</t>
   </si>
   <si>
-    <t xml:space="preserve">SERVICIOS ESPECIALIZADOS XOLOFLEX SA DE CV </t>
-  </si>
-  <si>
     <t>Mantenimiento a alarmas contra icendios  (o de alarmas)</t>
   </si>
   <si>
-    <t>UNIDAD DE SEGURIDAD PRIVADA OSIRIS, S.A. DE C.V.</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -150,27 +126,6 @@
     <t>PUE</t>
   </si>
   <si>
-    <t>LAN7008173R5</t>
-  </si>
-  <si>
-    <t>MSE061107IA8</t>
-  </si>
-  <si>
-    <t>TCM970625MB1</t>
-  </si>
-  <si>
-    <t>ACE0802066BA</t>
-  </si>
-  <si>
-    <t>APU140519728</t>
-  </si>
-  <si>
-    <t>CME160902CH3</t>
-  </si>
-  <si>
-    <t>GMA140516FN4</t>
-  </si>
-  <si>
     <t>99</t>
   </si>
   <si>
@@ -181,13 +136,43 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>NT Link Comunicaciones</t>
+  </si>
+  <si>
+    <t>NLC091211KC6</t>
+  </si>
+  <si>
+    <t>Arezzo Diseño Y Publicidad, S.A. De C.V.</t>
+  </si>
+  <si>
+    <t>Blake Ingeniería Integral, S.A. De C.V.</t>
+  </si>
+  <si>
+    <t>Centro Especializado en la Construcción Townsville, S.A. de C.V.</t>
+  </si>
+  <si>
+    <t>Consultores Administrativos Maruzzi, S.A. De C.V.</t>
+  </si>
+  <si>
+    <t>ADP171128RH1</t>
+  </si>
+  <si>
+    <t>BII180413413</t>
+  </si>
+  <si>
+    <t>CEC200207RJA</t>
+  </si>
+  <si>
+    <t>CAM160920N69</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +187,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -404,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -422,6 +413,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,56 +697,56 @@
   <dimension ref="A1:T62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="13" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="55.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="50.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" customWidth="1"/>
+    <col min="9" max="9" width="50.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
     <col min="15" max="15" width="42" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>3</v>
@@ -766,19 +758,19 @@
         <v>5</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="O1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="P1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="16" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -786,25 +778,25 @@
         <v>43760</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="H2" s="4">
         <v>80141600</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="4">
         <v>116030.85</v>
@@ -820,48 +812,48 @@
         <v>134595.78600000002</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="P2" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>43760</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1">
         <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1">
         <v>30161500</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1">
         <v>4269.26</v>
@@ -877,45 +869,45 @@
         <v>133713.22320000001</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>43760</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="H4" s="1">
         <v>80141500</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1">
         <v>156332.89000000001</v>
@@ -931,45 +923,45 @@
         <v>181346.15240000002</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5" s="11">
         <v>43760</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="H5" s="11">
         <v>92121702</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J5" s="11">
         <v>240045.29</v>
@@ -985,29 +977,29 @@
         <v>278452.53639999998</v>
       </c>
       <c r="N5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="P5" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0" right="0" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>